<commit_message>
find the max width of BT using CBT indexing
</commit_message>
<xml_diff>
--- a/DSA SHEET.xlsx
+++ b/DSA SHEET.xlsx
@@ -11,12 +11,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="138">
   <si>
     <t>Do NOT send any edit request to this sheet. Instead, make a copy of your own.</t>
   </si>
   <si>
     <t>DSA Series by Shradha Ma'am</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">Series Link : </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color rgb="FF1155CC"/>
+        <sz val="12.0"/>
+        <u/>
+      </rPr>
+      <t>DSA Series by Shradha Ma'am</t>
+    </r>
   </si>
   <si>
     <t>Mark as Done</t>
@@ -367,17 +387,68 @@
     <t>Reverse Linked List 2</t>
   </si>
   <si>
+    <t>LRU Cache</t>
+  </si>
+  <si>
     <t>Rotate a LL</t>
   </si>
   <si>
     <t>Reverse Nodes in K Groups</t>
+  </si>
+  <si>
+    <t>STACK &amp; QUEUE</t>
+  </si>
+  <si>
+    <t>Implement Stack using Queue</t>
+  </si>
+  <si>
+    <t>Implement Queue using Stack</t>
+  </si>
+  <si>
+    <t>Next Greater Element I</t>
+  </si>
+  <si>
+    <t>Valid Parenthesis</t>
+  </si>
+  <si>
+    <t>1st Non Repeating in Stream</t>
+  </si>
+  <si>
+    <t>Reverse 1st K Elements of Queue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time needed to Buy Tickets </t>
+  </si>
+  <si>
+    <t>Next Greater Element II</t>
+  </si>
+  <si>
+    <t>Previous Smaller Element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celebrity Problem </t>
+  </si>
+  <si>
+    <t>Get Min Element from Stack</t>
+  </si>
+  <si>
+    <t>Circular Tour / Gas Station</t>
+  </si>
+  <si>
+    <t>Rotten Oranges</t>
+  </si>
+  <si>
+    <t>Stock Span</t>
+  </si>
+  <si>
+    <t>Max Area in Histogram</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -397,6 +468,12 @@
       <b/>
       <sz val="14.0"/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10.0"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -517,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -539,6 +616,9 @@
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
@@ -554,34 +634,34 @@
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -590,31 +670,31 @@
     <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -629,11 +709,17 @@
     <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -899,8 +985,9 @@
         <v>1</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="4"/>
+      <c r="H2" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -947,27 +1034,27 @@
     </row>
     <row r="4">
       <c r="A4" s="1"/>
-      <c r="B4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="E4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="G4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="H4" s="12" t="s">
         <v>8</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1014,8 +1101,8 @@
       <c r="Y5" s="1"/>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="s">
-        <v>9</v>
+      <c r="A6" s="13" t="s">
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>0</v>
@@ -1024,19 +1111,19 @@
         <v>1.0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="F6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="G6" s="14" t="s">
         <v>14</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="1"/>
@@ -1064,22 +1151,22 @@
         <v>2.0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="F7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="15" t="s">
-        <v>16</v>
+      <c r="G7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1106,22 +1193,22 @@
         <v>3.0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="15" t="s">
-        <v>19</v>
+      <c r="G8" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>20</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1148,18 +1235,18 @@
         <v>4.0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="F9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="17"/>
+      <c r="G9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="18"/>
       <c r="I9" s="4"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1186,19 +1273,19 @@
         <v>5.0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="F10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="18" t="s">
-        <v>23</v>
+      <c r="G10" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>24</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="1"/>
@@ -1225,7 +1312,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="17"/>
+      <c r="H11" s="18"/>
       <c r="I11" s="4"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1252,19 +1339,19 @@
         <v>6.0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="15" t="s">
+      <c r="E12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>26</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="1"/>
@@ -1292,18 +1379,18 @@
         <v>7.0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="17"/>
+        <v>28</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="18"/>
       <c r="I13" s="4"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1330,19 +1417,19 @@
         <v>8.0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="15" t="s">
         <v>29</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="1"/>
@@ -1370,22 +1457,22 @@
         <v>9.0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="15" t="s">
         <v>31</v>
       </c>
+      <c r="E15" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="I15" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1412,22 +1499,22 @@
         <v>10.0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="20" t="s">
         <v>33</v>
       </c>
+      <c r="E16" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>34</v>
+      </c>
       <c r="I16" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1454,20 +1541,20 @@
         <v>11.0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="21"/>
+        <v>35</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="22"/>
       <c r="I17" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1493,21 +1580,21 @@
       <c r="C18" s="2">
         <v>12.0</v>
       </c>
-      <c r="D18" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="17"/>
+      <c r="D18" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="18"/>
       <c r="I18" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1534,22 +1621,22 @@
         <v>13.0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="15" t="s">
         <v>38</v>
       </c>
+      <c r="E19" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="I19" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -1576,20 +1663,20 @@
         <v>14.0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="15" t="s">
-        <v>40</v>
+      <c r="H20" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -1616,20 +1703,20 @@
         <v>15.0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="G21" s="4"/>
-      <c r="H21" s="15" t="s">
-        <v>42</v>
+      <c r="H21" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -1656,20 +1743,20 @@
         <v>16.0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>25</v>
+        <v>45</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="15" t="s">
-        <v>45</v>
+      <c r="H22" s="16" t="s">
+        <v>46</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -1696,20 +1783,20 @@
         <v>17.0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>25</v>
+        <v>48</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="G23" s="4"/>
-      <c r="H23" s="15" t="s">
-        <v>48</v>
+      <c r="H23" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1736,19 +1823,19 @@
         <v>18.0</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="18" t="s">
         <v>51</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="1"/>
@@ -1776,18 +1863,18 @@
         <v>19.0</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>25</v>
+        <v>53</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="G25" s="4"/>
-      <c r="H25" s="17"/>
+      <c r="H25" s="18"/>
       <c r="I25" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -1814,22 +1901,22 @@
         <v>20.0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" s="18" t="s">
         <v>54</v>
       </c>
+      <c r="E26" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>55</v>
+      </c>
       <c r="I26" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1855,7 +1942,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="17"/>
+      <c r="H27" s="18"/>
       <c r="I27" s="4"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -1882,20 +1969,20 @@
         <v>21.0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="23" t="s">
         <v>57</v>
       </c>
+      <c r="E28" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>58</v>
+      </c>
       <c r="G28" s="4"/>
-      <c r="H28" s="18" t="s">
-        <v>58</v>
+      <c r="H28" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -1922,17 +2009,19 @@
         <v>22.0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="G29" s="4"/>
-      <c r="H29" s="15" t="s">
+      <c r="E29" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="24" t="s">
         <v>62</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>63</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="1"/>
@@ -1960,20 +2049,22 @@
         <v>23.0</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="G30" s="4"/>
-      <c r="H30" s="15" t="s">
         <v>64</v>
       </c>
+      <c r="E30" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>65</v>
+      </c>
       <c r="I30" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -2000,18 +2091,18 @@
         <v>24.0</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="23" t="s">
-        <v>61</v>
+        <v>66</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>62</v>
       </c>
       <c r="G31" s="4"/>
-      <c r="H31" s="17"/>
+      <c r="H31" s="18"/>
       <c r="I31" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -2038,16 +2129,18 @@
         <v>25.0</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="17"/>
+        <v>67</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="18"/>
       <c r="I32" s="4"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -2074,7 +2167,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="1"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="17"/>
+      <c r="H33" s="18"/>
       <c r="I33" s="4"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -2101,7 +2194,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="1"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="17"/>
+      <c r="H34" s="18"/>
       <c r="I34" s="4"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -2121,8 +2214,8 @@
       <c r="Y34" s="1"/>
     </row>
     <row r="35">
-      <c r="A35" s="24" t="s">
-        <v>67</v>
+      <c r="A35" s="25" t="s">
+        <v>68</v>
       </c>
       <c r="B35" s="3" t="b">
         <v>0</v>
@@ -2130,20 +2223,20 @@
       <c r="C35" s="2">
         <v>1.0</v>
       </c>
-      <c r="D35" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="18" t="s">
+      <c r="D35" s="26" t="s">
         <v>69</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G35" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="19" t="s">
+        <v>70</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="1"/>
@@ -2170,19 +2263,19 @@
       <c r="C36" s="2">
         <v>2.0</v>
       </c>
-      <c r="D36" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="E36" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G36" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I36" s="28"/>
+      <c r="D36" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="29"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -2207,19 +2300,19 @@
       <c r="C37" s="2">
         <v>3.0</v>
       </c>
-      <c r="D37" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="E37" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H37" s="17"/>
+      <c r="D37" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="18"/>
       <c r="I37" s="4"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -2245,20 +2338,20 @@
       <c r="C38" s="2">
         <v>4.0</v>
       </c>
-      <c r="D38" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="E38" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H38" s="15" t="s">
+      <c r="D38" s="30" t="s">
         <v>73</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="1"/>
@@ -2285,17 +2378,17 @@
       <c r="C39" s="2">
         <v>5.0</v>
       </c>
-      <c r="D39" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="E39" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G39" s="16" t="s">
-        <v>13</v>
+      <c r="D39" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="1"/>
@@ -2322,20 +2415,20 @@
       <c r="C40" s="2">
         <v>6.0</v>
       </c>
-      <c r="D40" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E40" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G40" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" s="17" t="s">
+      <c r="D40" s="26" t="s">
         <v>76</v>
+      </c>
+      <c r="E40" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="1"/>
@@ -2359,21 +2452,21 @@
       <c r="B41" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C41" s="30">
+      <c r="C41" s="31">
         <v>7.0</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E41" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" s="23" t="s">
-        <v>61</v>
+        <v>78</v>
+      </c>
+      <c r="E41" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="24" t="s">
+        <v>62</v>
       </c>
       <c r="G41" s="4"/>
-      <c r="H41" s="18" t="s">
-        <v>78</v>
+      <c r="H41" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="1"/>
@@ -2401,7 +2494,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="1"/>
       <c r="G42" s="4"/>
-      <c r="H42" s="17"/>
+      <c r="H42" s="18"/>
       <c r="I42" s="4"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
@@ -2448,8 +2541,8 @@
       <c r="Y43" s="1"/>
     </row>
     <row r="44">
-      <c r="A44" s="31" t="s">
-        <v>79</v>
+      <c r="A44" s="32" t="s">
+        <v>80</v>
       </c>
       <c r="B44" s="3" t="b">
         <v>0</v>
@@ -2458,19 +2551,19 @@
         <v>1.0</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E44" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G44" s="16" t="s">
+      <c r="F44" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="H44" s="18" t="s">
-        <v>81</v>
+      <c r="G44" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="I44" s="4"/>
       <c r="J44" s="1"/>
@@ -2498,17 +2591,17 @@
         <v>2.0</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E45" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F45" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="E45" s="33" t="s">
         <v>12</v>
       </c>
+      <c r="F45" s="34" t="s">
+        <v>13</v>
+      </c>
       <c r="G45" s="4"/>
-      <c r="H45" s="18" t="s">
-        <v>83</v>
+      <c r="H45" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="I45" s="4"/>
       <c r="J45" s="1"/>
@@ -2536,17 +2629,17 @@
         <v>3.0</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E46" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F46" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46" s="33" t="s">
         <v>12</v>
       </c>
+      <c r="F46" s="34" t="s">
+        <v>13</v>
+      </c>
       <c r="G46" s="4"/>
-      <c r="H46" s="18" t="s">
-        <v>85</v>
+      <c r="H46" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="1"/>
@@ -2574,16 +2667,16 @@
         <v>4.0</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E47" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F47" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="G47" s="16" t="s">
-        <v>13</v>
+        <v>87</v>
+      </c>
+      <c r="E47" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G47" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="4"/>
@@ -2612,16 +2705,16 @@
         <v>5.0</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E48" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F48" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="G48" s="16" t="s">
-        <v>13</v>
+        <v>88</v>
+      </c>
+      <c r="E48" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G48" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="H48" s="5"/>
       <c r="I48" s="4"/>
@@ -2650,19 +2743,19 @@
         <v>6.0</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E49" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F49" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="G49" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H49" s="35" t="s">
-        <v>38</v>
+        <v>89</v>
+      </c>
+      <c r="E49" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" s="36" t="s">
+        <v>39</v>
       </c>
       <c r="I49" s="4"/>
       <c r="J49" s="1"/>
@@ -2686,20 +2779,20 @@
       <c r="B50" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C50" s="30">
+      <c r="C50" s="31">
         <v>7.0</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E50" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F50" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="G50" s="16" t="s">
-        <v>13</v>
+        <v>90</v>
+      </c>
+      <c r="E50" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="H50" s="5"/>
       <c r="I50" s="4"/>
@@ -2724,21 +2817,21 @@
       <c r="B51" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C51" s="30">
+      <c r="C51" s="31">
         <v>8.0</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E51" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51" s="34" t="s">
-        <v>25</v>
+        <v>91</v>
+      </c>
+      <c r="E51" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="35" t="s">
+        <v>26</v>
       </c>
       <c r="G51" s="4"/>
-      <c r="H51" s="35" t="s">
-        <v>91</v>
+      <c r="H51" s="36" t="s">
+        <v>92</v>
       </c>
       <c r="I51" s="4"/>
       <c r="J51" s="1"/>
@@ -2762,21 +2855,21 @@
       <c r="B52" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C52" s="30">
+      <c r="C52" s="31">
         <v>9.0</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E52" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" s="36" t="s">
-        <v>61</v>
+        <v>93</v>
+      </c>
+      <c r="E52" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="37" t="s">
+        <v>62</v>
       </c>
       <c r="G52" s="4"/>
-      <c r="H52" s="18" t="s">
-        <v>93</v>
+      <c r="H52" s="19" t="s">
+        <v>94</v>
       </c>
       <c r="I52" s="4"/>
       <c r="J52" s="1"/>
@@ -2800,17 +2893,17 @@
       <c r="B53" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C53" s="30">
+      <c r="C53" s="31">
         <v>10.0</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E53" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="36" t="s">
-        <v>61</v>
+        <v>95</v>
+      </c>
+      <c r="E53" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="37" t="s">
+        <v>62</v>
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="5"/>
@@ -2836,17 +2929,17 @@
       <c r="B54" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C54" s="30">
+      <c r="C54" s="31">
         <v>11.0</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F54" s="36" t="s">
-        <v>61</v>
+        <v>97</v>
+      </c>
+      <c r="F54" s="37" t="s">
+        <v>62</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="5"/>
@@ -2869,9 +2962,9 @@
       <c r="Y54" s="1"/>
     </row>
     <row r="55">
-      <c r="A55" s="37"/>
+      <c r="A55" s="38"/>
       <c r="B55" s="3"/>
-      <c r="C55" s="30"/>
+      <c r="C55" s="31"/>
       <c r="I55" s="4"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
@@ -2918,8 +3011,8 @@
       <c r="Y56" s="1"/>
     </row>
     <row r="57">
-      <c r="A57" s="38" t="s">
-        <v>97</v>
+      <c r="A57" s="39" t="s">
+        <v>98</v>
       </c>
       <c r="B57" s="3" t="b">
         <v>0</v>
@@ -2928,16 +3021,16 @@
         <v>1.0</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E57" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="G57" s="16" t="s">
-        <v>13</v>
+        <v>99</v>
+      </c>
+      <c r="E57" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G57" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="4"/>
@@ -2966,13 +3059,13 @@
         <v>2.0</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E58" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58" s="34" t="s">
-        <v>25</v>
+        <v>100</v>
+      </c>
+      <c r="E58" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" s="35" t="s">
+        <v>26</v>
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="5"/>
@@ -3002,16 +3095,16 @@
         <v>3.0</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E59" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F59" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="G59" s="16" t="s">
-        <v>13</v>
+        <v>101</v>
+      </c>
+      <c r="E59" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G59" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="H59" s="5"/>
       <c r="I59" s="4"/>
@@ -3040,13 +3133,13 @@
         <v>4.0</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E60" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F60" s="34" t="s">
-        <v>25</v>
+        <v>102</v>
+      </c>
+      <c r="E60" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="35" t="s">
+        <v>26</v>
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="5"/>
@@ -3076,13 +3169,13 @@
         <v>5.0</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E61" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F61" s="34" t="s">
-        <v>25</v>
+        <v>103</v>
+      </c>
+      <c r="E61" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="35" t="s">
+        <v>26</v>
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="5"/>
@@ -3112,16 +3205,16 @@
         <v>6.0</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E62" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F62" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="G62" s="16" t="s">
-        <v>13</v>
+        <v>104</v>
+      </c>
+      <c r="E62" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G62" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="H62" s="5"/>
       <c r="I62" s="4"/>
@@ -3146,20 +3239,20 @@
       <c r="B63" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C63" s="30">
+      <c r="C63" s="31">
         <v>7.0</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E63" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F63" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="G63" s="16" t="s">
-        <v>13</v>
+        <v>105</v>
+      </c>
+      <c r="E63" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G63" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="4"/>
@@ -3184,17 +3277,17 @@
       <c r="B64" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C64" s="30">
+      <c r="C64" s="31">
         <v>8.0</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E64" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F64" s="34" t="s">
-        <v>25</v>
+        <v>60</v>
+      </c>
+      <c r="E64" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="35" t="s">
+        <v>26</v>
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="5"/>
@@ -3220,20 +3313,20 @@
       <c r="B65" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C65" s="30">
+      <c r="C65" s="31">
         <v>9.0</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E65" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F65" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="G65" s="16" t="s">
-        <v>13</v>
+        <v>106</v>
+      </c>
+      <c r="E65" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="G65" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="H65" s="5"/>
       <c r="I65" s="4"/>
@@ -3258,20 +3351,20 @@
       <c r="B66" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C66" s="30">
+      <c r="C66" s="31">
         <v>10.0</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E66" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="G66" s="16" t="s">
-        <v>13</v>
+        <v>107</v>
+      </c>
+      <c r="E66" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="G66" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="H66" s="5"/>
       <c r="I66" s="4"/>
@@ -3296,17 +3389,17 @@
       <c r="B67" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C67" s="30">
+      <c r="C67" s="31">
         <v>11.0</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E67" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F67" s="36" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+      <c r="E67" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" s="37" t="s">
+        <v>62</v>
       </c>
       <c r="G67" s="4"/>
       <c r="H67" s="5"/>
@@ -3383,8 +3476,8 @@
       <c r="Y69" s="1"/>
     </row>
     <row r="70">
-      <c r="A70" s="38" t="s">
-        <v>107</v>
+      <c r="A70" s="39" t="s">
+        <v>108</v>
       </c>
       <c r="B70" s="3" t="b">
         <v>0</v>
@@ -3393,16 +3486,16 @@
         <v>1.0</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E70" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F70" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="E70" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G70" s="16" t="s">
+      <c r="F70" s="34" t="s">
         <v>13</v>
+      </c>
+      <c r="G70" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="H70" s="5"/>
       <c r="I70" s="4"/>
@@ -3431,15 +3524,17 @@
         <v>2.0</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E71" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F71" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E71" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G71" s="4"/>
+      <c r="F71" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G71" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H71" s="5"/>
       <c r="I71" s="4"/>
       <c r="J71" s="1"/>
@@ -3467,15 +3562,17 @@
         <v>3.0</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E72" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F72" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="E72" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G72" s="4"/>
+      <c r="F72" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G72" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H72" s="5"/>
       <c r="I72" s="4"/>
       <c r="J72" s="1"/>
@@ -3503,13 +3600,13 @@
         <v>4.0</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E73" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F73" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="E73" s="33" t="s">
         <v>12</v>
+      </c>
+      <c r="F73" s="34" t="s">
+        <v>13</v>
       </c>
       <c r="G73" s="4"/>
       <c r="H73" s="5"/>
@@ -3539,15 +3636,17 @@
         <v>5.0</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E74" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F74" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="E74" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G74" s="4"/>
+      <c r="F74" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G74" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H74" s="5"/>
       <c r="I74" s="4"/>
       <c r="J74" s="1"/>
@@ -3575,15 +3674,17 @@
         <v>6.0</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E75" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F75" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="G75" s="4"/>
+        <v>114</v>
+      </c>
+      <c r="E75" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F75" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G75" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H75" s="5"/>
       <c r="I75" s="4"/>
       <c r="J75" s="1"/>
@@ -3611,15 +3712,17 @@
         <v>7.0</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E76" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F76" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="G76" s="4"/>
+        <v>115</v>
+      </c>
+      <c r="E76" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F76" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G76" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H76" s="5"/>
       <c r="I76" s="4"/>
       <c r="J76" s="1"/>
@@ -3647,15 +3750,17 @@
         <v>8.0</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E77" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F77" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="G77" s="4"/>
+        <v>116</v>
+      </c>
+      <c r="E77" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F77" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G77" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H77" s="5"/>
       <c r="I77" s="4"/>
       <c r="J77" s="1"/>
@@ -3683,13 +3788,13 @@
         <v>9.0</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E78" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F78" s="34" t="s">
-        <v>25</v>
+        <v>117</v>
+      </c>
+      <c r="E78" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F78" s="35" t="s">
+        <v>26</v>
       </c>
       <c r="G78" s="4"/>
       <c r="H78" s="5"/>
@@ -3719,13 +3824,13 @@
         <v>10.0</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E79" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F79" s="34" t="s">
-        <v>25</v>
+        <v>118</v>
+      </c>
+      <c r="E79" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79" s="35" t="s">
+        <v>26</v>
       </c>
       <c r="G79" s="4"/>
       <c r="H79" s="5"/>
@@ -3751,19 +3856,21 @@
       <c r="B80" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80" s="31">
         <v>11.0</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E80" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F80" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="G80" s="4"/>
+        <v>119</v>
+      </c>
+      <c r="E80" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G80" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H80" s="5"/>
       <c r="I80" s="4"/>
       <c r="J80" s="1"/>
@@ -3787,17 +3894,17 @@
       <c r="B81" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C81" s="31">
         <v>12.0</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E81" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F81" s="36" t="s">
-        <v>61</v>
+        <v>120</v>
+      </c>
+      <c r="E81" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81" s="35" t="s">
+        <v>26</v>
       </c>
       <c r="G81" s="4"/>
       <c r="H81" s="5"/>
@@ -3820,13 +3927,24 @@
       <c r="Y81" s="1"/>
     </row>
     <row r="82">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="4"/>
+      <c r="B82" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C82" s="31">
+        <v>13.0</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E82" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F82" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="G82" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H82" s="5"/>
       <c r="I82" s="4"/>
       <c r="J82" s="1"/>
@@ -3901,13 +4019,27 @@
       <c r="Y84" s="1"/>
     </row>
     <row r="85">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="4"/>
+      <c r="A85" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="B85" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C85" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E85" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F85" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G85" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H85" s="5"/>
       <c r="I85" s="4"/>
       <c r="J85" s="1"/>
@@ -3928,13 +4060,24 @@
       <c r="Y85" s="1"/>
     </row>
     <row r="86">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="4"/>
+      <c r="B86" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C86" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E86" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F86" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G86" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H86" s="5"/>
       <c r="I86" s="4"/>
       <c r="J86" s="1"/>
@@ -3955,13 +4098,24 @@
       <c r="Y86" s="1"/>
     </row>
     <row r="87">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="4"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="4"/>
+      <c r="B87" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C87" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D87" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="E87" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F87" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G87" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H87" s="5"/>
       <c r="I87" s="4"/>
       <c r="J87" s="1"/>
@@ -3982,13 +4136,24 @@
       <c r="Y87" s="1"/>
     </row>
     <row r="88">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="1"/>
-      <c r="G88" s="4"/>
+      <c r="B88" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C88" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E88" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F88" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G88" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H88" s="5"/>
       <c r="I88" s="4"/>
       <c r="J88" s="1"/>
@@ -4009,13 +4174,24 @@
       <c r="Y88" s="1"/>
     </row>
     <row r="89">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="4"/>
-      <c r="F89" s="1"/>
-      <c r="G89" s="4"/>
+      <c r="B89" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C89" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E89" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F89" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G89" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H89" s="5"/>
       <c r="I89" s="4"/>
       <c r="J89" s="1"/>
@@ -4036,12 +4212,21 @@
       <c r="Y89" s="1"/>
     </row>
     <row r="90">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="4"/>
-      <c r="F90" s="1"/>
+      <c r="B90" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C90" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E90" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F90" s="34" t="s">
+        <v>13</v>
+      </c>
       <c r="G90" s="4"/>
       <c r="H90" s="5"/>
       <c r="I90" s="4"/>
@@ -4063,12 +4248,21 @@
       <c r="Y90" s="1"/>
     </row>
     <row r="91">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="1"/>
+      <c r="B91" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C91" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E91" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91" s="34" t="s">
+        <v>13</v>
+      </c>
       <c r="G91" s="4"/>
       <c r="H91" s="5"/>
       <c r="I91" s="4"/>
@@ -4090,13 +4284,24 @@
       <c r="Y91" s="1"/>
     </row>
     <row r="92">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="1"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="1"/>
-      <c r="G92" s="4"/>
+      <c r="B92" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C92" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="D92" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E92" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G92" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H92" s="5"/>
       <c r="I92" s="4"/>
       <c r="J92" s="1"/>
@@ -4117,13 +4322,24 @@
       <c r="Y92" s="1"/>
     </row>
     <row r="93">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="1"/>
-      <c r="E93" s="4"/>
-      <c r="F93" s="1"/>
-      <c r="G93" s="4"/>
+      <c r="B93" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C93" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="D93" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="E93" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F93" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G93" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H93" s="5"/>
       <c r="I93" s="4"/>
       <c r="J93" s="1"/>
@@ -4144,13 +4360,24 @@
       <c r="Y93" s="1"/>
     </row>
     <row r="94">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="4"/>
-      <c r="F94" s="1"/>
-      <c r="G94" s="4"/>
+      <c r="B94" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C94" s="41">
+        <v>10.0</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E94" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F94" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G94" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H94" s="5"/>
       <c r="I94" s="4"/>
       <c r="J94" s="1"/>
@@ -4171,13 +4398,24 @@
       <c r="Y94" s="1"/>
     </row>
     <row r="95">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="1"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="1"/>
-      <c r="G95" s="4"/>
+      <c r="B95" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C95" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E95" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F95" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G95" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H95" s="5"/>
       <c r="I95" s="4"/>
       <c r="J95" s="1"/>
@@ -4198,13 +4436,24 @@
       <c r="Y95" s="1"/>
     </row>
     <row r="96">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="1"/>
-      <c r="E96" s="4"/>
-      <c r="F96" s="1"/>
-      <c r="G96" s="4"/>
+      <c r="B96" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C96" s="2">
+        <v>12.0</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E96" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F96" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G96" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H96" s="5"/>
       <c r="I96" s="4"/>
       <c r="J96" s="1"/>
@@ -4225,12 +4474,21 @@
       <c r="Y96" s="1"/>
     </row>
     <row r="97">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="1"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="1"/>
+      <c r="B97" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C97" s="2">
+        <v>13.0</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E97" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F97" s="35" t="s">
+        <v>26</v>
+      </c>
       <c r="G97" s="4"/>
       <c r="H97" s="5"/>
       <c r="I97" s="4"/>
@@ -4252,13 +4510,24 @@
       <c r="Y97" s="1"/>
     </row>
     <row r="98">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="1"/>
-      <c r="E98" s="4"/>
-      <c r="F98" s="1"/>
-      <c r="G98" s="4"/>
+      <c r="B98" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C98" s="2">
+        <v>14.0</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E98" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F98" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G98" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H98" s="5"/>
       <c r="I98" s="4"/>
       <c r="J98" s="1"/>
@@ -4279,13 +4548,24 @@
       <c r="Y98" s="1"/>
     </row>
     <row r="99">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="1"/>
-      <c r="E99" s="4"/>
-      <c r="F99" s="1"/>
-      <c r="G99" s="4"/>
+      <c r="B99" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C99" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E99" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F99" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="G99" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H99" s="5"/>
       <c r="I99" s="4"/>
       <c r="J99" s="1"/>
@@ -28687,115 +28967,157 @@
       <c r="Y1002" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="A70:A82"/>
+    <mergeCell ref="A85:A99"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="D2:F2"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="A6:A32"/>
     <mergeCell ref="A35:A41"/>
     <mergeCell ref="A44:A54"/>
     <mergeCell ref="A57:A67"/>
-    <mergeCell ref="A70:A81"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E6"/>
-    <hyperlink r:id="rId2" ref="G6"/>
-    <hyperlink r:id="rId3" ref="E7"/>
-    <hyperlink r:id="rId4" ref="G7"/>
-    <hyperlink r:id="rId5" ref="E8"/>
-    <hyperlink r:id="rId6" ref="G8"/>
-    <hyperlink r:id="rId7" ref="E9"/>
-    <hyperlink r:id="rId8" ref="G9"/>
-    <hyperlink r:id="rId9" ref="E10"/>
-    <hyperlink r:id="rId10" ref="G10"/>
-    <hyperlink r:id="rId11" ref="E12"/>
-    <hyperlink r:id="rId12" ref="G12"/>
-    <hyperlink r:id="rId13" ref="E13"/>
-    <hyperlink r:id="rId14" ref="G13"/>
-    <hyperlink r:id="rId15" ref="E14"/>
-    <hyperlink r:id="rId16" ref="G14"/>
-    <hyperlink r:id="rId17" ref="E15"/>
-    <hyperlink r:id="rId18" ref="G15"/>
-    <hyperlink r:id="rId19" ref="E16"/>
-    <hyperlink r:id="rId20" ref="G16"/>
-    <hyperlink r:id="rId21" ref="E17"/>
-    <hyperlink r:id="rId22" ref="G17"/>
-    <hyperlink r:id="rId23" ref="E18"/>
-    <hyperlink r:id="rId24" ref="G18"/>
-    <hyperlink r:id="rId25" ref="E19"/>
-    <hyperlink r:id="rId26" ref="G19"/>
-    <hyperlink r:id="rId27" ref="E20"/>
-    <hyperlink r:id="rId28" ref="E21"/>
-    <hyperlink r:id="rId29" ref="E22"/>
-    <hyperlink r:id="rId30" ref="E23"/>
-    <hyperlink r:id="rId31" ref="E24"/>
-    <hyperlink r:id="rId32" ref="G24"/>
-    <hyperlink r:id="rId33" ref="E25"/>
-    <hyperlink r:id="rId34" ref="E26"/>
-    <hyperlink r:id="rId35" ref="G26"/>
-    <hyperlink r:id="rId36" ref="E28"/>
-    <hyperlink r:id="rId37" ref="E29"/>
-    <hyperlink r:id="rId38" ref="E30"/>
-    <hyperlink r:id="rId39" ref="E31"/>
-    <hyperlink r:id="rId40" ref="E32"/>
-    <hyperlink r:id="rId41" ref="E35"/>
-    <hyperlink r:id="rId42" ref="G35"/>
-    <hyperlink r:id="rId43" ref="E36"/>
-    <hyperlink r:id="rId44" ref="G36"/>
-    <hyperlink r:id="rId45" ref="E37"/>
-    <hyperlink r:id="rId46" ref="G37"/>
-    <hyperlink r:id="rId47" ref="E38"/>
-    <hyperlink r:id="rId48" ref="G38"/>
-    <hyperlink r:id="rId49" ref="E39"/>
-    <hyperlink r:id="rId50" ref="G39"/>
-    <hyperlink r:id="rId51" ref="E40"/>
-    <hyperlink r:id="rId52" ref="G40"/>
-    <hyperlink r:id="rId53" ref="E41"/>
-    <hyperlink r:id="rId54" ref="E44"/>
-    <hyperlink r:id="rId55" ref="G44"/>
-    <hyperlink r:id="rId56" ref="E45"/>
-    <hyperlink r:id="rId57" ref="E46"/>
-    <hyperlink r:id="rId58" ref="E47"/>
-    <hyperlink r:id="rId59" ref="G47"/>
-    <hyperlink r:id="rId60" ref="E48"/>
-    <hyperlink r:id="rId61" ref="G48"/>
-    <hyperlink r:id="rId62" ref="E49"/>
-    <hyperlink r:id="rId63" ref="G49"/>
-    <hyperlink r:id="rId64" ref="E50"/>
-    <hyperlink r:id="rId65" ref="G50"/>
-    <hyperlink r:id="rId66" ref="E51"/>
-    <hyperlink r:id="rId67" ref="E52"/>
-    <hyperlink r:id="rId68" ref="E53"/>
-    <hyperlink r:id="rId69" ref="E57"/>
-    <hyperlink r:id="rId70" ref="G57"/>
-    <hyperlink r:id="rId71" ref="E58"/>
-    <hyperlink r:id="rId72" ref="E59"/>
-    <hyperlink r:id="rId73" ref="G59"/>
-    <hyperlink r:id="rId74" ref="E60"/>
-    <hyperlink r:id="rId75" ref="E61"/>
-    <hyperlink r:id="rId76" ref="E62"/>
-    <hyperlink r:id="rId77" ref="G62"/>
-    <hyperlink r:id="rId78" ref="E63"/>
-    <hyperlink r:id="rId79" ref="G63"/>
-    <hyperlink r:id="rId80" ref="E64"/>
-    <hyperlink r:id="rId81" ref="E65"/>
-    <hyperlink r:id="rId82" ref="G65"/>
-    <hyperlink r:id="rId83" ref="E66"/>
-    <hyperlink r:id="rId84" ref="G66"/>
-    <hyperlink r:id="rId85" ref="E67"/>
-    <hyperlink r:id="rId86" ref="E70"/>
-    <hyperlink r:id="rId87" ref="G70"/>
-    <hyperlink r:id="rId88" ref="E71"/>
-    <hyperlink r:id="rId89" ref="E72"/>
-    <hyperlink r:id="rId90" ref="E73"/>
-    <hyperlink r:id="rId91" ref="E74"/>
-    <hyperlink r:id="rId92" ref="E75"/>
-    <hyperlink r:id="rId93" ref="E76"/>
-    <hyperlink r:id="rId94" ref="E77"/>
-    <hyperlink r:id="rId95" ref="E78"/>
-    <hyperlink r:id="rId96" ref="E79"/>
-    <hyperlink r:id="rId97" ref="E80"/>
-    <hyperlink r:id="rId98" ref="E81"/>
+    <hyperlink r:id="rId1" ref="H2"/>
+    <hyperlink r:id="rId2" ref="E6"/>
+    <hyperlink r:id="rId3" ref="G6"/>
+    <hyperlink r:id="rId4" ref="E7"/>
+    <hyperlink r:id="rId5" ref="G7"/>
+    <hyperlink r:id="rId6" ref="E8"/>
+    <hyperlink r:id="rId7" ref="G8"/>
+    <hyperlink r:id="rId8" ref="E9"/>
+    <hyperlink r:id="rId9" ref="G9"/>
+    <hyperlink r:id="rId10" ref="E10"/>
+    <hyperlink r:id="rId11" ref="G10"/>
+    <hyperlink r:id="rId12" ref="E12"/>
+    <hyperlink r:id="rId13" ref="G12"/>
+    <hyperlink r:id="rId14" ref="E13"/>
+    <hyperlink r:id="rId15" ref="G13"/>
+    <hyperlink r:id="rId16" ref="E14"/>
+    <hyperlink r:id="rId17" ref="G14"/>
+    <hyperlink r:id="rId18" ref="E15"/>
+    <hyperlink r:id="rId19" ref="G15"/>
+    <hyperlink r:id="rId20" ref="E16"/>
+    <hyperlink r:id="rId21" ref="G16"/>
+    <hyperlink r:id="rId22" ref="E17"/>
+    <hyperlink r:id="rId23" ref="G17"/>
+    <hyperlink r:id="rId24" ref="E18"/>
+    <hyperlink r:id="rId25" ref="G18"/>
+    <hyperlink r:id="rId26" ref="E19"/>
+    <hyperlink r:id="rId27" ref="G19"/>
+    <hyperlink r:id="rId28" ref="E20"/>
+    <hyperlink r:id="rId29" ref="E21"/>
+    <hyperlink r:id="rId30" ref="E22"/>
+    <hyperlink r:id="rId31" ref="E23"/>
+    <hyperlink r:id="rId32" ref="E24"/>
+    <hyperlink r:id="rId33" ref="G24"/>
+    <hyperlink r:id="rId34" ref="E25"/>
+    <hyperlink r:id="rId35" ref="E26"/>
+    <hyperlink r:id="rId36" ref="G26"/>
+    <hyperlink r:id="rId37" ref="E28"/>
+    <hyperlink r:id="rId38" ref="E29"/>
+    <hyperlink r:id="rId39" ref="G29"/>
+    <hyperlink r:id="rId40" ref="E30"/>
+    <hyperlink r:id="rId41" ref="G30"/>
+    <hyperlink r:id="rId42" ref="E31"/>
+    <hyperlink r:id="rId43" ref="E32"/>
+    <hyperlink r:id="rId44" ref="G32"/>
+    <hyperlink r:id="rId45" ref="E35"/>
+    <hyperlink r:id="rId46" ref="G35"/>
+    <hyperlink r:id="rId47" ref="E36"/>
+    <hyperlink r:id="rId48" ref="G36"/>
+    <hyperlink r:id="rId49" ref="E37"/>
+    <hyperlink r:id="rId50" ref="G37"/>
+    <hyperlink r:id="rId51" ref="E38"/>
+    <hyperlink r:id="rId52" ref="G38"/>
+    <hyperlink r:id="rId53" ref="E39"/>
+    <hyperlink r:id="rId54" ref="G39"/>
+    <hyperlink r:id="rId55" ref="E40"/>
+    <hyperlink r:id="rId56" ref="G40"/>
+    <hyperlink r:id="rId57" ref="E41"/>
+    <hyperlink r:id="rId58" ref="E44"/>
+    <hyperlink r:id="rId59" ref="G44"/>
+    <hyperlink r:id="rId60" ref="E45"/>
+    <hyperlink r:id="rId61" ref="E46"/>
+    <hyperlink r:id="rId62" ref="E47"/>
+    <hyperlink r:id="rId63" ref="G47"/>
+    <hyperlink r:id="rId64" ref="E48"/>
+    <hyperlink r:id="rId65" ref="G48"/>
+    <hyperlink r:id="rId66" ref="E49"/>
+    <hyperlink r:id="rId67" ref="G49"/>
+    <hyperlink r:id="rId68" ref="E50"/>
+    <hyperlink r:id="rId69" ref="G50"/>
+    <hyperlink r:id="rId70" ref="E51"/>
+    <hyperlink r:id="rId71" ref="E52"/>
+    <hyperlink r:id="rId72" ref="E53"/>
+    <hyperlink r:id="rId73" ref="E57"/>
+    <hyperlink r:id="rId74" ref="G57"/>
+    <hyperlink r:id="rId75" ref="E58"/>
+    <hyperlink r:id="rId76" ref="E59"/>
+    <hyperlink r:id="rId77" ref="G59"/>
+    <hyperlink r:id="rId78" ref="E60"/>
+    <hyperlink r:id="rId79" ref="E61"/>
+    <hyperlink r:id="rId80" ref="E62"/>
+    <hyperlink r:id="rId81" ref="G62"/>
+    <hyperlink r:id="rId82" ref="E63"/>
+    <hyperlink r:id="rId83" ref="G63"/>
+    <hyperlink r:id="rId84" ref="E64"/>
+    <hyperlink r:id="rId85" ref="E65"/>
+    <hyperlink r:id="rId86" ref="G65"/>
+    <hyperlink r:id="rId87" ref="E66"/>
+    <hyperlink r:id="rId88" ref="G66"/>
+    <hyperlink r:id="rId89" ref="E67"/>
+    <hyperlink r:id="rId90" ref="E70"/>
+    <hyperlink r:id="rId91" ref="G70"/>
+    <hyperlink r:id="rId92" ref="E71"/>
+    <hyperlink r:id="rId93" ref="G71"/>
+    <hyperlink r:id="rId94" ref="E72"/>
+    <hyperlink r:id="rId95" ref="G72"/>
+    <hyperlink r:id="rId96" ref="E73"/>
+    <hyperlink r:id="rId97" ref="E74"/>
+    <hyperlink r:id="rId98" ref="G74"/>
+    <hyperlink r:id="rId99" ref="E75"/>
+    <hyperlink r:id="rId100" ref="G75"/>
+    <hyperlink r:id="rId101" ref="E76"/>
+    <hyperlink r:id="rId102" ref="G76"/>
+    <hyperlink r:id="rId103" ref="E77"/>
+    <hyperlink r:id="rId104" ref="G77"/>
+    <hyperlink r:id="rId105" ref="E78"/>
+    <hyperlink r:id="rId106" ref="E79"/>
+    <hyperlink r:id="rId107" ref="E80"/>
+    <hyperlink r:id="rId108" ref="G80"/>
+    <hyperlink r:id="rId109" ref="E81"/>
+    <hyperlink r:id="rId110" ref="E82"/>
+    <hyperlink r:id="rId111" ref="G82"/>
+    <hyperlink r:id="rId112" ref="E85"/>
+    <hyperlink r:id="rId113" ref="G85"/>
+    <hyperlink r:id="rId114" ref="E86"/>
+    <hyperlink r:id="rId115" ref="G86"/>
+    <hyperlink r:id="rId116" ref="E87"/>
+    <hyperlink r:id="rId117" ref="G87"/>
+    <hyperlink r:id="rId118" ref="E88"/>
+    <hyperlink r:id="rId119" ref="G88"/>
+    <hyperlink r:id="rId120" ref="E89"/>
+    <hyperlink r:id="rId121" ref="G89"/>
+    <hyperlink r:id="rId122" ref="E90"/>
+    <hyperlink r:id="rId123" ref="E91"/>
+    <hyperlink r:id="rId124" ref="E92"/>
+    <hyperlink r:id="rId125" ref="G92"/>
+    <hyperlink r:id="rId126" ref="E93"/>
+    <hyperlink r:id="rId127" ref="G93"/>
+    <hyperlink r:id="rId128" ref="E94"/>
+    <hyperlink r:id="rId129" ref="G94"/>
+    <hyperlink r:id="rId130" ref="E95"/>
+    <hyperlink r:id="rId131" ref="G95"/>
+    <hyperlink r:id="rId132" ref="E96"/>
+    <hyperlink r:id="rId133" ref="G96"/>
+    <hyperlink r:id="rId134" ref="E97"/>
+    <hyperlink r:id="rId135" ref="E98"/>
+    <hyperlink r:id="rId136" ref="G98"/>
+    <hyperlink r:id="rId137" ref="E99"/>
+    <hyperlink r:id="rId138" ref="G99"/>
   </hyperlinks>
-  <drawing r:id="rId99"/>
+  <drawing r:id="rId139"/>
 </worksheet>
 </file>
</xml_diff>